<commit_message>
fix: corrindo script do python, no qual estava removendo o título da coluna
</commit_message>
<xml_diff>
--- a/FormattedResult.xlsx
+++ b/FormattedResult.xlsx
@@ -495,25 +495,41 @@
           <t>Secção</t>
         </is>
       </c>
-      <c r="C1" s="10" t="inlineStr"/>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>Código Divisão</t>
+        </is>
+      </c>
       <c r="D1" s="10" t="inlineStr">
         <is>
           <t>Divisão</t>
         </is>
       </c>
-      <c r="E1" s="10" t="inlineStr"/>
+      <c r="E1" s="10" t="inlineStr">
+        <is>
+          <t>Código Grupo</t>
+        </is>
+      </c>
       <c r="F1" s="10" t="inlineStr">
         <is>
           <t>Grupo</t>
         </is>
       </c>
-      <c r="G1" s="10" t="inlineStr"/>
+      <c r="G1" s="10" t="inlineStr">
+        <is>
+          <t>Código Classe</t>
+        </is>
+      </c>
       <c r="H1" s="10" t="inlineStr">
         <is>
           <t>Classe</t>
         </is>
       </c>
-      <c r="I1" s="10" t="inlineStr"/>
+      <c r="I1" s="10" t="inlineStr">
+        <is>
+          <t>Código Subclasse</t>
+        </is>
+      </c>
       <c r="J1" s="10" t="inlineStr">
         <is>
           <t>Subclasse</t>

</xml_diff>